<commit_message>
engadido campo Huso no modelo de datos
</commit_message>
<xml_diff>
--- a/scripts/modelo_de_datos_GL_v1_0.xlsx
+++ b/scripts/modelo_de_datos_GL_v1_0.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t xml:space="preserve">NOME</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t xml:space="preserve">PLATAFORMAS VINCULADAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUSO (29, 30,...)</t>
   </si>
   <si>
     <t xml:space="preserve">id</t>
@@ -269,10 +272,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -341,6 +344,12 @@
         <v>9</v>
       </c>
       <c r="B10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -364,24 +373,24 @@
       <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="6" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="8" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="8" width="8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1405,24 +1414,24 @@
       <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="6" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="8" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="8" width="8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2446,24 +2455,24 @@
       <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="6" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="8" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="8" width="8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3599,24 +3608,24 @@
       <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="6" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="8" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="8" width="8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4752,24 +4761,24 @@
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="6" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="7" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="8" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="8" width="8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -5802,13 +5811,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -5842,13 +5851,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -5882,13 +5891,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>